<commit_message>
Additions/Revisions to eProcedures.03, dConfiguration.03, dConfiguration.07 - Procedures.xlsx Category name change:  OLD: Blood Administration, NEW: Fluid Administration Addition: 225372007 - Total parenteral nutrition (regime/therapy)
</commit_message>
<xml_diff>
--- a/SuggestedLists/eProcedures.03, dConfiguration.03, dConfiguration.07 - Procedures.xlsx
+++ b/SuggestedLists/eProcedures.03, dConfiguration.03, dConfiguration.07 - Procedures.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmann\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1095" windowWidth="15315" windowHeight="9975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="3528"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Change Log" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
   <si>
     <t>NEMSIS TAC Version 3 - Procedures (eProcedures.03, dConfiguration.03, dConfiguration.07) - SNOMED CT Hierarchy Suggested List</t>
   </si>
@@ -756,9 +761,6 @@
     <t>Catheterization of umbilical vein (procedure)</t>
   </si>
   <si>
-    <t>Blood Administration</t>
-  </si>
-  <si>
     <t>Albumin</t>
   </si>
   <si>
@@ -811,13 +813,31 @@
   </si>
   <si>
     <t>Needle Decompression</t>
+  </si>
+  <si>
+    <t>Additions/Revisions - 10/4/2018</t>
+  </si>
+  <si>
+    <t>Category name change:  OLD: Blood Administration, NEW: Fluid Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addition: 225372007 - Total parenteral nutrition (regime/therapy) </t>
+  </si>
+  <si>
+    <t>Fluid Administration</t>
+  </si>
+  <si>
+    <t>Total parenteral nutrition (regime/therapy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total parenteral nutrition </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,6 +908,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -963,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1077,6 +1104,8 @@
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,6 +1115,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1134,7 +1166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1169,7 +1201,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1378,22 +1410,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +1433,7 @@
       <c r="C1" s="23"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -1409,7 +1441,7 @@
       <c r="C2" s="16"/>
       <c r="D2" s="26"/>
     </row>
-    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1423,13 +1455,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
       <c r="B4" s="36"/>
       <c r="C4" s="37"/>
       <c r="D4" s="36"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1437,7 +1469,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="14" t="s">
         <v>7</v>
@@ -1449,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="14" t="s">
         <v>9</v>
@@ -1461,7 +1493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="14" t="s">
         <v>11</v>
@@ -1473,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="14" t="s">
         <v>13</v>
@@ -1485,7 +1517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="14" t="s">
         <v>15</v>
@@ -1497,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="14" t="s">
         <v>17</v>
@@ -1509,7 +1541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="14" t="s">
         <v>19</v>
@@ -1521,7 +1553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="14" t="s">
         <v>21</v>
@@ -1533,7 +1565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="14" t="s">
         <v>23</v>
@@ -1545,7 +1577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="14" t="s">
         <v>25</v>
@@ -1557,7 +1589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="14" t="s">
         <v>27</v>
@@ -1569,7 +1601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="14" t="s">
         <v>29</v>
@@ -1581,7 +1613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="14" t="s">
         <v>31</v>
@@ -1593,7 +1625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="14" t="s">
         <v>33</v>
@@ -1605,7 +1637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="14" t="s">
         <v>35</v>
@@ -1617,13 +1649,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="37"/>
       <c r="D21" s="36"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1631,7 +1663,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="14" t="s">
         <v>38</v>
@@ -1643,7 +1675,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="14" t="s">
         <v>40</v>
@@ -1655,7 +1687,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="14" t="s">
         <v>42</v>
@@ -1667,7 +1699,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="14" t="s">
         <v>44</v>
@@ -1679,7 +1711,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="14" t="s">
         <v>46</v>
@@ -1691,10 +1723,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C28" s="10">
         <v>241689008</v>
@@ -1703,7 +1735,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="14" t="s">
         <v>48</v>
@@ -1715,7 +1747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="14" t="s">
         <v>50</v>
@@ -1727,7 +1759,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="14" t="s">
         <v>52</v>
@@ -1739,7 +1771,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="14" t="s">
         <v>54</v>
@@ -1751,7 +1783,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="15" t="s">
         <v>56</v>
@@ -1763,7 +1795,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="14" t="s">
         <v>60</v>
@@ -1775,7 +1807,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="14" t="s">
         <v>62</v>
@@ -1787,7 +1819,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
       <c r="B36" s="18" t="s">
         <v>64</v>
@@ -1799,7 +1831,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="18" t="s">
         <v>66</v>
@@ -1811,7 +1843,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="14" t="s">
         <v>68</v>
@@ -1823,7 +1855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="14" t="s">
         <v>70</v>
@@ -1835,7 +1867,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="14" t="s">
         <v>72</v>
@@ -1847,7 +1879,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="14" t="s">
         <v>75</v>
@@ -1859,7 +1891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="14" t="s">
         <v>77</v>
@@ -1871,7 +1903,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="14" t="s">
         <v>79</v>
@@ -1883,13 +1915,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" s="36"/>
       <c r="C44" s="37"/>
       <c r="D44" s="36"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>81</v>
       </c>
@@ -1897,7 +1929,7 @@
       <c r="C45" s="10"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="14" t="s">
         <v>82</v>
@@ -1909,7 +1941,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="14" t="s">
         <v>84</v>
@@ -1921,7 +1953,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="14" t="s">
         <v>86</v>
@@ -1933,13 +1965,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="35"/>
       <c r="B49" s="36"/>
       <c r="C49" s="37"/>
       <c r="D49" s="36"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>88</v>
       </c>
@@ -1947,7 +1979,7 @@
       <c r="C50" s="10"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="14" t="s">
         <v>89</v>
@@ -1959,7 +1991,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="14" t="s">
         <v>91</v>
@@ -1971,7 +2003,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="14" t="s">
         <v>93</v>
@@ -1983,7 +2015,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="17" t="s">
         <v>95</v>
@@ -1995,7 +2027,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="17" t="s">
         <v>97</v>
@@ -2007,7 +2039,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="17" t="s">
         <v>99</v>
@@ -2019,7 +2051,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="17" t="s">
         <v>101</v>
@@ -2031,7 +2063,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="17" t="s">
         <v>103</v>
@@ -2043,7 +2075,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="17" t="s">
         <v>106</v>
@@ -2055,7 +2087,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="17" t="s">
         <v>108</v>
@@ -2067,7 +2099,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="17" t="s">
         <v>110</v>
@@ -2079,7 +2111,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="17" t="s">
         <v>112</v>
@@ -2091,7 +2123,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="17" t="s">
         <v>114</v>
@@ -2103,7 +2135,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="17" t="s">
         <v>116</v>
@@ -2115,7 +2147,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="17" t="s">
         <v>118</v>
@@ -2127,7 +2159,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="17" t="s">
         <v>120</v>
@@ -2139,13 +2171,13 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="35"/>
       <c r="B67" s="36"/>
       <c r="C67" s="37"/>
       <c r="D67" s="36"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>122</v>
       </c>
@@ -2153,7 +2185,7 @@
       <c r="C68" s="10"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="6" t="s">
         <v>123</v>
@@ -2165,7 +2197,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="6" t="s">
         <v>125</v>
@@ -2177,10 +2209,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C71" s="10">
         <v>182705007</v>
@@ -2189,13 +2221,13 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="35"/>
       <c r="B72" s="36"/>
       <c r="C72" s="37"/>
       <c r="D72" s="36"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>128</v>
       </c>
@@ -2203,7 +2235,7 @@
       <c r="C73" s="10"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="14" t="s">
         <v>129</v>
@@ -2215,7 +2247,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="14" t="s">
         <v>131</v>
@@ -2227,13 +2259,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="35"/>
       <c r="B76" s="36"/>
       <c r="C76" s="37"/>
       <c r="D76" s="36"/>
     </row>
-    <row r="77" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>133</v>
       </c>
@@ -2241,7 +2273,7 @@
       <c r="C77" s="10"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="14" t="s">
         <v>134</v>
@@ -2253,7 +2285,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="14" t="s">
         <v>136</v>
@@ -2265,7 +2297,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="14" t="s">
         <v>138</v>
@@ -2277,7 +2309,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="14" t="s">
         <v>140</v>
@@ -2289,7 +2321,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="6" t="s">
         <v>142</v>
@@ -2301,7 +2333,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="14" t="s">
         <v>144</v>
@@ -2313,7 +2345,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="18" t="s">
         <v>146</v>
@@ -2325,7 +2357,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="18" t="s">
         <v>148</v>
@@ -2337,7 +2369,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="16" t="s">
         <v>150</v>
@@ -2349,7 +2381,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="14" t="s">
         <v>152</v>
@@ -2361,13 +2393,13 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="35"/>
       <c r="B88" s="36"/>
       <c r="C88" s="37"/>
       <c r="D88" s="36"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>154</v>
       </c>
@@ -2375,7 +2407,7 @@
       <c r="C89" s="10"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="14" t="s">
         <v>155</v>
@@ -2387,7 +2419,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="14" t="s">
         <v>157</v>
@@ -2399,7 +2431,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="14" t="s">
         <v>159</v>
@@ -2411,7 +2443,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="14" t="s">
         <v>161</v>
@@ -2423,13 +2455,13 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="35"/>
       <c r="B94" s="36"/>
       <c r="C94" s="38"/>
       <c r="D94" s="36"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>163</v>
       </c>
@@ -2437,7 +2469,7 @@
       <c r="C95" s="10"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="19" t="s">
         <v>164</v>
@@ -2449,7 +2481,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="7" t="s">
         <v>166</v>
@@ -2461,7 +2493,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="14" t="s">
         <v>168</v>
@@ -2473,7 +2505,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="14" t="s">
         <v>170</v>
@@ -2485,7 +2517,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="8"/>
       <c r="B100" s="7" t="s">
         <v>172</v>
@@ -2497,7 +2529,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="8"/>
       <c r="B101" s="7" t="s">
         <v>175</v>
@@ -2509,7 +2541,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="14" t="s">
         <v>177</v>
@@ -2521,7 +2553,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="14" t="s">
         <v>179</v>
@@ -2533,7 +2565,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="14" t="s">
         <v>181</v>
@@ -2545,7 +2577,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="14" t="s">
         <v>183</v>
@@ -2557,7 +2589,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="14" t="s">
         <v>185</v>
@@ -2569,13 +2601,13 @@
         <v>186</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
       <c r="C107" s="37"/>
       <c r="D107" s="36"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>187</v>
       </c>
@@ -2583,7 +2615,7 @@
       <c r="C108" s="10"/>
       <c r="D108" s="6"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="14" t="s">
         <v>188</v>
@@ -2595,7 +2627,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="14" t="s">
         <v>190</v>
@@ -2607,13 +2639,13 @@
         <v>191</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="35"/>
       <c r="B111" s="36"/>
       <c r="C111" s="37"/>
       <c r="D111" s="36"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>192</v>
       </c>
@@ -2621,7 +2653,7 @@
       <c r="C112" s="10"/>
       <c r="D112" s="6"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="14" t="s">
         <v>193</v>
@@ -2633,7 +2665,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="14" t="s">
         <v>195</v>
@@ -2645,7 +2677,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="14" t="s">
         <v>197</v>
@@ -2657,7 +2689,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="14" t="s">
         <v>199</v>
@@ -2669,7 +2701,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="14" t="s">
         <v>201</v>
@@ -2681,7 +2713,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="14" t="s">
         <v>203</v>
@@ -2693,7 +2725,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="14" t="s">
         <v>205</v>
@@ -2705,13 +2737,13 @@
         <v>206</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="35"/>
       <c r="B120" s="36"/>
       <c r="C120" s="37"/>
       <c r="D120" s="36"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>207</v>
       </c>
@@ -2719,7 +2751,7 @@
       <c r="C121" s="10"/>
       <c r="D121" s="6"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="17" t="s">
         <v>208</v>
@@ -2731,7 +2763,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="14" t="s">
         <v>210</v>
@@ -2743,7 +2775,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="17" t="s">
         <v>212</v>
@@ -2755,7 +2787,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="17" t="s">
         <v>214</v>
@@ -2767,7 +2799,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="17" t="s">
         <v>216</v>
@@ -2779,7 +2811,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="17" t="s">
         <v>218</v>
@@ -2791,7 +2823,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="17" t="s">
         <v>220</v>
@@ -2803,7 +2835,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="14" t="s">
         <v>222</v>
@@ -2815,7 +2847,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="17" t="s">
         <v>224</v>
@@ -2827,7 +2859,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="14" t="s">
         <v>226</v>
@@ -2839,7 +2871,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="32"/>
       <c r="B132" s="6" t="s">
         <v>228</v>
@@ -2851,7 +2883,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="17" t="s">
         <v>230</v>
@@ -2863,7 +2895,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="18" t="s">
         <v>232</v>
@@ -2875,7 +2907,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="6" t="s">
         <v>234</v>
@@ -2887,7 +2919,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="6" t="s">
         <v>236</v>
@@ -2899,7 +2931,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="6" t="s">
         <v>238</v>
@@ -2911,7 +2943,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="6" t="s">
         <v>240</v>
@@ -2923,7 +2955,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="B139" s="6" t="s">
         <v>242</v>
@@ -2935,7 +2967,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="B140" s="6" t="s">
         <v>244</v>
@@ -2947,113 +2979,125 @@
         <v>245</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="35"/>
       <c r="B141" s="39"/>
       <c r="C141" s="40"/>
       <c r="D141" s="39"/>
     </row>
-    <row r="142" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="B142" s="33"/>
       <c r="C142" s="34"/>
       <c r="D142" s="33"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="6" t="s">
+    <row r="143" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="3"/>
+      <c r="B143" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C143" s="11">
+        <v>225372007</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B144" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C144" s="10">
+        <v>116865006</v>
+      </c>
+      <c r="D144" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C143" s="10">
-        <v>116865006</v>
-      </c>
-      <c r="D143" s="6" t="s">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="8"/>
+      <c r="B145" s="14" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="8"/>
-      <c r="B144" s="14" t="s">
+      <c r="C145" s="10">
+        <v>116762002</v>
+      </c>
+      <c r="D145" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C144" s="10">
-        <v>116762002</v>
-      </c>
-      <c r="D144" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="3"/>
-      <c r="B145" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="C145" s="10">
-        <v>116795008</v>
-      </c>
-      <c r="D145" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="3"/>
       <c r="B146" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C146" s="10">
-        <v>116861002</v>
+        <v>116795008</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="3"/>
       <c r="B147" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C147" s="10">
-        <v>426518006</v>
+        <v>116861002</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="3"/>
       <c r="B148" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="C148" s="10">
+        <v>426518006</v>
+      </c>
+      <c r="D148" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="3"/>
+      <c r="B149" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C149" s="10">
+        <v>71493000</v>
+      </c>
+      <c r="D149" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C148" s="10">
-        <v>71493000</v>
-      </c>
-      <c r="D148" s="6" t="s">
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="8"/>
+      <c r="B150" s="20" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="8"/>
-      <c r="B149" s="20" t="s">
+      <c r="C150" s="10">
+        <v>180208003</v>
+      </c>
+      <c r="D150" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="C149" s="10">
-        <v>180208003</v>
-      </c>
-      <c r="D149" s="21" t="s">
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="3"/>
+      <c r="B151" s="14" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="3"/>
-      <c r="B150" s="14" t="s">
+      <c r="C151" s="10">
+        <v>33389009</v>
+      </c>
+      <c r="D151" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="C150" s="10">
-        <v>33389009</v>
-      </c>
-      <c r="D150" s="6" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3067,12 +3111,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3083,7 +3145,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final updates/bug fixes: Update to suggested lists Update to add effectiveDate attribute to StateDataSet Bug fix to add CorrelationId to Chest and Lung Groups in eExam section.
</commit_message>
<xml_diff>
--- a/SuggestedLists/eProcedures.03, dConfiguration.03, dConfiguration.07 - Procedures.xlsx
+++ b/SuggestedLists/eProcedures.03, dConfiguration.03, dConfiguration.07 - Procedures.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Users\cmann\DAILY FILES\GRANTS\NEMSIS\V3\V3_5_0\Suggested Lists\Refined Suggested Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Users\jehlers\v3 Suggested Lists\Final Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F60A1CE4-861B-4E7B-92C4-AF27C98B69ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15012" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15020" windowHeight="9290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recommendation" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
   <si>
     <t>Count of Events</t>
   </si>
@@ -404,9 +405,6 @@
     <t>Holding patient (procedure)</t>
   </si>
   <si>
-    <t>Total count of event</t>
-  </si>
-  <si>
     <t>SNOMED</t>
   </si>
   <si>
@@ -557,6 +555,9 @@
     <t>Capillary refill</t>
   </si>
   <si>
+    <t>New (I think the capillary blood glucose has been misused as this)</t>
+  </si>
+  <si>
     <t>IV fluids</t>
   </si>
   <si>
@@ -743,6 +744,9 @@
     <t>Total events with Procedure listed</t>
   </si>
   <si>
+    <t>Not sure where to put this</t>
+  </si>
+  <si>
     <t>Intubation, combitube</t>
   </si>
   <si>
@@ -833,22 +837,23 @@
     <t>Includes 89003005 Oral temperature</t>
   </si>
   <si>
-    <t>Revised Draft Suggested List (eProcedure.03: Procedure)</t>
+    <t>eProcedure.03: Procedure Suggested List</t>
   </si>
   <si>
     <t>Record Date Range Evaluated: 01/01/2017 through 07/01/2019</t>
+  </si>
+  <si>
+    <t>Total count of events</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -894,35 +899,12 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -950,7 +932,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1137,67 +1119,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1232,6 +1158,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1310,6 +1239,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1406,14 +1338,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1427,7 +1362,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1454,120 +1389,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1845,92 +1683,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BA138"/>
+  <dimension ref="A1:K139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="37" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="38" customWidth="1"/>
     <col min="4" max="4" width="87" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="87" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="94.6640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="10"/>
-    <col min="9" max="9" width="5.88671875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="59.109375" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="10"/>
+    <col min="5" max="5" width="12.7265625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="94.7265625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="10"/>
+    <col min="9" max="9" width="5.81640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="22.7265625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="59.1796875" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B1" s="112" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="B1" s="90" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D2" s="11"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D3" s="11"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E4" s="114" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="E4" s="75" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="D5" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="89">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="14">
         <v>37063795</v>
       </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D6" s="15" t="s">
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="90">
+      <c r="E6" s="17">
         <v>703598</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="15" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="90">
+      <c r="E7" s="17">
         <v>1656431</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="71" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D8" s="74" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="113">
+      <c r="E8" s="91">
         <f>E5-E6-E7</f>
         <v>34703766</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1938,12 +1776,12 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="91" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1953,28 +1791,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="63"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="66"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="65"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="18">
+        <v>135</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="19">
         <v>18629005</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="20">
         <v>21722</v>
       </c>
       <c r="F11" s="8">
@@ -1982,17 +1820,17 @@
         <v>6.2592630436708228E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" s="18">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="19">
         <v>386358000</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="93">
+      <c r="E12" s="20">
         <v>7728</v>
       </c>
       <c r="F12" s="8">
@@ -2000,17 +1838,17 @@
         <v>2.226847656822029E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="18">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="19">
         <v>431393006</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="93">
+      <c r="E13" s="20">
         <v>5840</v>
       </c>
       <c r="F13" s="8">
@@ -2018,17 +1856,17 @@
         <v>1.682814481863438E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="19">
         <v>103744005</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="93">
+      <c r="E14" s="20">
         <f>39527+8189</f>
         <v>47716</v>
       </c>
@@ -2037,20 +1875,20 @@
         <v>1.3749516406951338E-3</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="18">
+        <v>138</v>
+      </c>
+      <c r="C15" s="19">
         <v>56251003</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="93">
+      <c r="E15" s="20">
         <v>22642</v>
       </c>
       <c r="F15" s="8">
@@ -2058,36 +1896,36 @@
         <v>6.5243639551972542E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="C16" s="18">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C16" s="19">
         <v>57485005</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E16" s="93">
+      <c r="E16" s="20">
         <v>11876</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>3.4221069840085941E-4</v>
       </c>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="18">
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="19">
         <v>371907003</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="93">
+      <c r="E17" s="20">
         <v>97181</v>
       </c>
       <c r="F17" s="8">
@@ -2095,17 +1933,17 @@
         <v>2.8003012698967597E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="19">
         <v>371908008</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="93">
+      <c r="E18" s="20">
         <v>21632</v>
       </c>
       <c r="F18" s="8">
@@ -2113,286 +1951,286 @@
         <v>6.2333292588475839E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="63"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="66"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="65"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="68"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="18">
+        <v>250</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="19">
         <v>230040009</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="93">
+      <c r="E20" s="20">
         <v>106158</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="23">
         <f t="shared" ref="F20:F27" si="1">E20/$E$8</f>
         <v>3.0589763658503228E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="18">
+        <v>144</v>
+      </c>
+      <c r="C21" s="19">
         <v>425447009</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="93">
+      <c r="E21" s="20">
         <v>135646</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="23">
         <f t="shared" si="1"/>
         <v>3.9086824179254782E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C22" s="51">
+      <c r="B22" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="53">
         <v>243140006</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="95">
+      <c r="E22" s="54">
         <v>24727</v>
       </c>
-      <c r="F22" s="67">
+      <c r="F22" s="69">
         <f t="shared" si="1"/>
         <v>7.1251633036022665E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="77"/>
-      <c r="B23" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="C23" s="81">
+    <row r="23" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="80"/>
+      <c r="B23" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C23" s="84">
         <v>284029005</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="D23" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="96">
+      <c r="E23" s="85">
         <v>15938</v>
       </c>
-      <c r="F23" s="83">
+      <c r="F23" s="86">
         <f>E23/$E$8</f>
         <v>4.5925851390307324E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="C24" s="44">
+      <c r="B24" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C24" s="46">
         <v>23690002</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="97">
+      <c r="E24" s="47">
         <v>873</v>
       </c>
-      <c r="F24" s="36">
+      <c r="F24" s="37">
         <f>E24/$E$8</f>
         <v>2.5155771278540779E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="18">
+        <v>146</v>
+      </c>
+      <c r="C25" s="19">
         <v>182692007</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="93">
+      <c r="E25" s="20">
         <v>56690</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="23">
         <f t="shared" si="1"/>
         <v>1.633540290699286E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" s="18">
+        <v>145</v>
+      </c>
+      <c r="C26" s="19">
         <v>7443007</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="93">
+      <c r="E26" s="20">
         <v>68082</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="23">
         <f t="shared" si="1"/>
         <v>1.9618043759285376E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27" s="18">
+        <v>147</v>
+      </c>
+      <c r="C27" s="19">
         <v>232664002</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="93">
+      <c r="E27" s="20">
         <v>22807</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="23">
         <f t="shared" si="1"/>
         <v>6.5719092273731905E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="63"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="66"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="65"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="68"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="69">
+      <c r="C29" s="71">
         <v>243142003</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="93">
+      <c r="E29" s="20">
         <v>5715</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="23">
         <f t="shared" ref="F29:F39" si="2">E29/$E$8</f>
         <v>1.6467953362756077E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="24">
         <v>47545007</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="99">
+      <c r="E30" s="7">
         <f>110015+5381</f>
         <v>115396</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="23">
         <f t="shared" si="2"/>
         <v>3.3251722594026252E-3</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="69">
+        <v>163</v>
+      </c>
+      <c r="C31" s="71">
         <v>225718003</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="93">
+      <c r="E31" s="20">
         <v>17467</v>
       </c>
       <c r="F31" s="8">
         <f t="shared" si="2"/>
         <v>5.0331713278610739E-4</v>
       </c>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="C32" s="34">
+      <c r="B32" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32" s="35">
         <v>425543005</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="100">
+      <c r="E32" s="36">
         <v>107784</v>
       </c>
-      <c r="F32" s="70">
+      <c r="F32" s="73">
         <f t="shared" si="2"/>
         <v>3.1058300704309726E-3</v>
       </c>
-      <c r="G32" s="85"/>
-    </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G32" s="88"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C33" s="44">
+        <v>240</v>
+      </c>
+      <c r="C33" s="46">
         <v>429705000</v>
       </c>
-      <c r="D33" s="84" t="s">
+      <c r="D33" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="101">
+      <c r="E33" s="87">
         <v>2233</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="37">
         <f t="shared" si="2"/>
         <v>6.4344601678100293E-5</v>
       </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-    </row>
-    <row r="34" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G33" s="14"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C34" s="23">
+        <v>241</v>
+      </c>
+      <c r="C34" s="24">
         <v>424979004</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="99">
+      <c r="E34" s="7">
         <f>8706+2677</f>
         <v>11383</v>
       </c>
@@ -2400,21 +2238,21 @@
         <f t="shared" si="2"/>
         <v>3.2800474738101912E-4</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G34" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C35" s="23">
+        <v>150</v>
+      </c>
+      <c r="C35" s="24">
         <v>232674004</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="99">
+      <c r="E35" s="7">
         <f>103619+4897+2260</f>
         <v>110776</v>
       </c>
@@ -2422,692 +2260,279 @@
         <f t="shared" si="2"/>
         <v>3.1920454973100036E-3</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G35" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C36" s="23">
+        <v>242</v>
+      </c>
+      <c r="C36" s="24">
         <v>241689008</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="99">
+      <c r="E36" s="7">
         <v>8988</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="2"/>
         <v>2.5899206443473597E-4</v>
       </c>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B37" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C37" s="23">
+        <v>243</v>
+      </c>
+      <c r="C37" s="24">
         <v>427753009</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="99">
+      <c r="E37" s="7">
         <v>22001</v>
       </c>
       <c r="F37" s="8">
         <f t="shared" si="2"/>
         <v>6.3396577766228603E-4</v>
       </c>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B38" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C38" s="23">
+        <v>162</v>
+      </c>
+      <c r="C38" s="24">
         <v>45851008</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="99">
+      <c r="E38" s="7">
         <v>6029</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" si="2"/>
         <v>1.7372754299922378E-4</v>
       </c>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="24">
         <v>385857005</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="99">
+      <c r="E39" s="7">
         <v>69662</v>
       </c>
       <c r="F39" s="8">
         <f t="shared" si="2"/>
         <v>2.0073325759515552E-3</v>
       </c>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A40" s="63"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="122"/>
-      <c r="I40" s="122"/>
-      <c r="J40" s="122"/>
-      <c r="K40" s="122"/>
-      <c r="L40" s="122"/>
-      <c r="M40" s="122"/>
-      <c r="N40" s="122"/>
-      <c r="O40" s="122"/>
-      <c r="P40" s="122"/>
-      <c r="Q40" s="122"/>
-      <c r="R40" s="122"/>
-      <c r="S40" s="122"/>
-      <c r="T40" s="122"/>
-      <c r="U40" s="122"/>
-      <c r="V40" s="122"/>
-      <c r="W40" s="122"/>
-      <c r="X40" s="122"/>
-      <c r="Y40" s="122"/>
-      <c r="Z40" s="122"/>
-      <c r="AA40" s="122"/>
-      <c r="AB40" s="122"/>
-      <c r="AC40" s="122"/>
-      <c r="AD40" s="122"/>
-      <c r="AE40" s="122"/>
-      <c r="AF40" s="122"/>
-      <c r="AG40" s="122"/>
-      <c r="AH40" s="122"/>
-      <c r="AI40" s="122"/>
-      <c r="AJ40" s="122"/>
-      <c r="AK40" s="122"/>
-      <c r="AL40" s="122"/>
-      <c r="AM40" s="122"/>
-      <c r="AN40" s="122"/>
-      <c r="AO40" s="122"/>
-      <c r="AP40" s="122"/>
-      <c r="AQ40" s="122"/>
-      <c r="AR40" s="122"/>
-      <c r="AS40" s="122"/>
-      <c r="AT40" s="122"/>
-      <c r="AU40" s="122"/>
-      <c r="AV40" s="122"/>
-      <c r="AW40" s="122"/>
-      <c r="AX40" s="122"/>
-      <c r="AY40" s="122"/>
-      <c r="AZ40" s="122"/>
-      <c r="BA40" s="122"/>
-    </row>
-    <row r="41" spans="1:53" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="73" t="s">
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="65"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="76" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C41" s="60">
+      <c r="C41" s="62">
         <v>408994004</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="102">
+      <c r="E41" s="63">
         <f>53901+156683+8447</f>
         <v>219031</v>
       </c>
-      <c r="F41" s="57">
+      <c r="F41" s="59">
         <f t="shared" ref="F41:F49" si="3">E41/$E$8</f>
         <v>6.3114475817984709E-3</v>
       </c>
-      <c r="G41" s="120" t="s">
-        <v>254</v>
-      </c>
-      <c r="H41" s="120"/>
-      <c r="I41" s="120"/>
-      <c r="J41" s="120"/>
-      <c r="K41" s="120"/>
-      <c r="L41" s="120"/>
-      <c r="M41" s="120"/>
-      <c r="N41" s="120"/>
-      <c r="O41" s="120"/>
-      <c r="P41" s="120"/>
-      <c r="Q41" s="120"/>
-      <c r="R41" s="120"/>
-      <c r="S41" s="120"/>
-      <c r="T41" s="120"/>
-      <c r="U41" s="120"/>
-      <c r="V41" s="120"/>
-      <c r="W41" s="120"/>
-      <c r="X41" s="120"/>
-      <c r="Y41" s="120"/>
-      <c r="Z41" s="120"/>
-      <c r="AA41" s="120"/>
-      <c r="AB41" s="120"/>
-      <c r="AC41" s="120"/>
-      <c r="AD41" s="120"/>
-      <c r="AE41" s="120"/>
-      <c r="AF41" s="120"/>
-      <c r="AG41" s="120"/>
-      <c r="AH41" s="120"/>
-      <c r="AI41" s="120"/>
-      <c r="AJ41" s="120"/>
-      <c r="AK41" s="120"/>
-      <c r="AL41" s="120"/>
-      <c r="AM41" s="120"/>
-      <c r="AN41" s="120"/>
-      <c r="AO41" s="120"/>
-      <c r="AP41" s="120"/>
-      <c r="AQ41" s="120"/>
-      <c r="AR41" s="120"/>
-      <c r="AS41" s="120"/>
-      <c r="AT41" s="120"/>
-      <c r="AU41" s="120"/>
-      <c r="AV41" s="120"/>
-      <c r="AW41" s="120"/>
-      <c r="AX41" s="120"/>
-      <c r="AY41" s="120"/>
-      <c r="AZ41" s="120"/>
-      <c r="BA41" s="120"/>
-    </row>
-    <row r="42" spans="1:53" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="73"/>
+      <c r="G41" s="89" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="76"/>
       <c r="B42" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C42" s="60">
+      <c r="C42" s="62">
         <v>422618004</v>
       </c>
-      <c r="D42" s="61" t="s">
+      <c r="D42" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="102">
+      <c r="E42" s="63">
         <v>3592058</v>
       </c>
-      <c r="F42" s="57">
+      <c r="F42" s="59">
         <f t="shared" si="3"/>
         <v>0.10350628804954483</v>
       </c>
-      <c r="G42" s="121"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="120"/>
-      <c r="J42" s="120"/>
-      <c r="K42" s="120"/>
-      <c r="L42" s="120"/>
-      <c r="M42" s="120"/>
-      <c r="N42" s="120"/>
-      <c r="O42" s="120"/>
-      <c r="P42" s="120"/>
-      <c r="Q42" s="120"/>
-      <c r="R42" s="120"/>
-      <c r="S42" s="120"/>
-      <c r="T42" s="120"/>
-      <c r="U42" s="120"/>
-      <c r="V42" s="120"/>
-      <c r="W42" s="120"/>
-      <c r="X42" s="120"/>
-      <c r="Y42" s="120"/>
-      <c r="Z42" s="120"/>
-      <c r="AA42" s="120"/>
-      <c r="AB42" s="120"/>
-      <c r="AC42" s="120"/>
-      <c r="AD42" s="120"/>
-      <c r="AE42" s="120"/>
-      <c r="AF42" s="120"/>
-      <c r="AG42" s="120"/>
-      <c r="AH42" s="120"/>
-      <c r="AI42" s="120"/>
-      <c r="AJ42" s="120"/>
-      <c r="AK42" s="120"/>
-      <c r="AL42" s="120"/>
-      <c r="AM42" s="120"/>
-      <c r="AN42" s="120"/>
-      <c r="AO42" s="120"/>
-      <c r="AP42" s="120"/>
-      <c r="AQ42" s="120"/>
-      <c r="AR42" s="120"/>
-      <c r="AS42" s="120"/>
-      <c r="AT42" s="120"/>
-      <c r="AU42" s="120"/>
-      <c r="AV42" s="120"/>
-      <c r="AW42" s="120"/>
-      <c r="AX42" s="120"/>
-      <c r="AY42" s="120"/>
-      <c r="AZ42" s="120"/>
-      <c r="BA42" s="120"/>
-    </row>
-    <row r="43" spans="1:53" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="73"/>
+      <c r="G42" s="89"/>
+    </row>
+    <row r="43" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="76"/>
       <c r="B43" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C43" s="60">
+      <c r="C43" s="62">
         <v>315639002</v>
       </c>
-      <c r="D43" s="61" t="s">
+      <c r="D43" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="102">
+      <c r="E43" s="63">
         <v>63922</v>
       </c>
-      <c r="F43" s="57">
+      <c r="F43" s="59">
         <f t="shared" si="3"/>
         <v>1.8419326594122378E-3</v>
       </c>
-      <c r="G43" s="120"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="120"/>
-      <c r="J43" s="120"/>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120"/>
-      <c r="O43" s="120"/>
-      <c r="P43" s="120"/>
-      <c r="Q43" s="120"/>
-      <c r="R43" s="120"/>
-      <c r="S43" s="120"/>
-      <c r="T43" s="120"/>
-      <c r="U43" s="120"/>
-      <c r="V43" s="120"/>
-      <c r="W43" s="120"/>
-      <c r="X43" s="120"/>
-      <c r="Y43" s="120"/>
-      <c r="Z43" s="120"/>
-      <c r="AA43" s="120"/>
-      <c r="AB43" s="120"/>
-      <c r="AC43" s="120"/>
-      <c r="AD43" s="120"/>
-      <c r="AE43" s="120"/>
-      <c r="AF43" s="120"/>
-      <c r="AG43" s="120"/>
-      <c r="AH43" s="120"/>
-      <c r="AI43" s="120"/>
-      <c r="AJ43" s="120"/>
-      <c r="AK43" s="120"/>
-      <c r="AL43" s="120"/>
-      <c r="AM43" s="120"/>
-      <c r="AN43" s="120"/>
-      <c r="AO43" s="120"/>
-      <c r="AP43" s="120"/>
-      <c r="AQ43" s="120"/>
-      <c r="AR43" s="120"/>
-      <c r="AS43" s="120"/>
-      <c r="AT43" s="120"/>
-      <c r="AU43" s="120"/>
-      <c r="AV43" s="120"/>
-      <c r="AW43" s="120"/>
-      <c r="AX43" s="120"/>
-      <c r="AY43" s="120"/>
-      <c r="AZ43" s="120"/>
-      <c r="BA43" s="120"/>
-    </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A44" s="74"/>
+      <c r="G43" s="89"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="77"/>
       <c r="B44" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="75">
+      <c r="C44" s="78">
         <v>225398001</v>
       </c>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="103">
+      <c r="E44" s="61">
         <f>6953+6317</f>
         <v>13270</v>
       </c>
-      <c r="F44" s="117">
+      <c r="F44" s="59">
         <f t="shared" si="3"/>
         <v>3.8237924956040795E-4</v>
       </c>
-      <c r="G44" s="121" t="s">
-        <v>255</v>
-      </c>
-      <c r="H44" s="120"/>
-      <c r="I44" s="122"/>
-      <c r="J44" s="122"/>
-      <c r="K44" s="122"/>
-      <c r="L44" s="122"/>
-      <c r="M44" s="122"/>
-      <c r="N44" s="122"/>
-      <c r="O44" s="122"/>
-      <c r="P44" s="122"/>
-      <c r="Q44" s="122"/>
-      <c r="R44" s="122"/>
-      <c r="S44" s="122"/>
-      <c r="T44" s="122"/>
-      <c r="U44" s="122"/>
-      <c r="V44" s="122"/>
-      <c r="W44" s="122"/>
-      <c r="X44" s="122"/>
-      <c r="Y44" s="122"/>
-      <c r="Z44" s="122"/>
-      <c r="AA44" s="122"/>
-      <c r="AB44" s="122"/>
-      <c r="AC44" s="122"/>
-      <c r="AD44" s="122"/>
-      <c r="AE44" s="122"/>
-      <c r="AF44" s="122"/>
-      <c r="AG44" s="122"/>
-      <c r="AH44" s="122"/>
-      <c r="AI44" s="122"/>
-      <c r="AJ44" s="122"/>
-      <c r="AK44" s="122"/>
-      <c r="AL44" s="122"/>
-      <c r="AM44" s="122"/>
-      <c r="AN44" s="122"/>
-      <c r="AO44" s="122"/>
-      <c r="AP44" s="122"/>
-      <c r="AQ44" s="122"/>
-      <c r="AR44" s="122"/>
-      <c r="AS44" s="122"/>
-      <c r="AT44" s="122"/>
-      <c r="AU44" s="122"/>
-      <c r="AV44" s="122"/>
-      <c r="AW44" s="122"/>
-      <c r="AX44" s="122"/>
-      <c r="AY44" s="122"/>
-      <c r="AZ44" s="122"/>
-      <c r="BA44" s="122"/>
-    </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A45" s="74"/>
+      <c r="G44" s="89" t="s">
+        <v>256</v>
+      </c>
+      <c r="H44" s="60"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="77"/>
       <c r="B45" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="39">
+      <c r="C45" s="41">
         <v>423850004</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E45" s="93">
+      <c r="E45" s="20">
         <v>6790</v>
       </c>
-      <c r="F45" s="118">
+      <c r="F45" s="8">
         <f t="shared" si="3"/>
         <v>1.9565599883309494E-4</v>
       </c>
-      <c r="G45" s="119"/>
-      <c r="H45" s="122"/>
-      <c r="I45" s="122"/>
-      <c r="J45" s="122"/>
-      <c r="K45" s="122"/>
-      <c r="L45" s="122"/>
-      <c r="M45" s="122"/>
-      <c r="N45" s="122"/>
-      <c r="O45" s="122"/>
-      <c r="P45" s="122"/>
-      <c r="Q45" s="122"/>
-      <c r="R45" s="122"/>
-      <c r="S45" s="122"/>
-      <c r="T45" s="122"/>
-      <c r="U45" s="122"/>
-      <c r="V45" s="122"/>
-      <c r="W45" s="122"/>
-      <c r="X45" s="122"/>
-      <c r="Y45" s="122"/>
-      <c r="Z45" s="122"/>
-      <c r="AA45" s="122"/>
-      <c r="AB45" s="122"/>
-      <c r="AC45" s="122"/>
-      <c r="AD45" s="122"/>
-      <c r="AE45" s="122"/>
-      <c r="AF45" s="122"/>
-      <c r="AG45" s="122"/>
-      <c r="AH45" s="122"/>
-      <c r="AI45" s="122"/>
-      <c r="AJ45" s="122"/>
-      <c r="AK45" s="122"/>
-      <c r="AL45" s="122"/>
-      <c r="AM45" s="122"/>
-      <c r="AN45" s="122"/>
-      <c r="AO45" s="122"/>
-      <c r="AP45" s="122"/>
-      <c r="AQ45" s="122"/>
-      <c r="AR45" s="122"/>
-      <c r="AS45" s="122"/>
-      <c r="AT45" s="122"/>
-      <c r="AU45" s="122"/>
-      <c r="AV45" s="122"/>
-      <c r="AW45" s="122"/>
-      <c r="AX45" s="122"/>
-      <c r="AY45" s="122"/>
-      <c r="AZ45" s="122"/>
-      <c r="BA45" s="122"/>
-    </row>
-    <row r="46" spans="1:53" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="73"/>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="76"/>
       <c r="B46" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C46" s="76">
+      <c r="C46" s="79">
         <v>386053000</v>
       </c>
-      <c r="D46" s="56" t="s">
+      <c r="D46" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="E46" s="104">
+      <c r="E46" s="58">
         <v>1312424</v>
       </c>
-      <c r="F46" s="57">
+      <c r="F46" s="59">
         <f t="shared" si="3"/>
         <v>3.7817912903170221E-2</v>
       </c>
-      <c r="G46" s="121"/>
-      <c r="H46" s="120"/>
-      <c r="I46" s="120"/>
-      <c r="J46" s="120"/>
-      <c r="K46" s="120"/>
-      <c r="L46" s="120"/>
-      <c r="M46" s="120"/>
-      <c r="N46" s="120"/>
-      <c r="O46" s="120"/>
-      <c r="P46" s="120"/>
-      <c r="Q46" s="120"/>
-      <c r="R46" s="120"/>
-      <c r="S46" s="120"/>
-      <c r="T46" s="120"/>
-      <c r="U46" s="120"/>
-      <c r="V46" s="120"/>
-      <c r="W46" s="120"/>
-      <c r="X46" s="120"/>
-      <c r="Y46" s="120"/>
-      <c r="Z46" s="120"/>
-      <c r="AA46" s="120"/>
-      <c r="AB46" s="120"/>
-      <c r="AC46" s="120"/>
-      <c r="AD46" s="120"/>
-      <c r="AE46" s="120"/>
-      <c r="AF46" s="120"/>
-      <c r="AG46" s="120"/>
-      <c r="AH46" s="120"/>
-      <c r="AI46" s="120"/>
-      <c r="AJ46" s="120"/>
-      <c r="AK46" s="120"/>
-      <c r="AL46" s="120"/>
-      <c r="AM46" s="120"/>
-      <c r="AN46" s="120"/>
-      <c r="AO46" s="120"/>
-      <c r="AP46" s="120"/>
-      <c r="AQ46" s="120"/>
-      <c r="AR46" s="120"/>
-      <c r="AS46" s="120"/>
-      <c r="AT46" s="120"/>
-      <c r="AU46" s="120"/>
-      <c r="AV46" s="120"/>
-      <c r="AW46" s="120"/>
-      <c r="AX46" s="120"/>
-      <c r="AY46" s="120"/>
-      <c r="AZ46" s="120"/>
-      <c r="BA46" s="120"/>
-    </row>
-    <row r="47" spans="1:53" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="73"/>
+      <c r="G46" s="89"/>
+    </row>
+    <row r="47" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="76"/>
       <c r="B47" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="C47" s="76">
+      <c r="C47" s="79">
         <v>270352002</v>
       </c>
-      <c r="D47" s="56" t="s">
+      <c r="D47" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="104">
+      <c r="E47" s="58">
         <f>13431+17996</f>
         <v>31427</v>
       </c>
-      <c r="F47" s="57">
+      <c r="F47" s="59">
         <f t="shared" si="3"/>
         <v>9.0557895071099776E-4</v>
       </c>
-      <c r="G47" s="121" t="s">
-        <v>256</v>
-      </c>
-      <c r="H47" s="120"/>
-      <c r="I47" s="120"/>
-      <c r="J47" s="120"/>
-      <c r="K47" s="120"/>
-      <c r="L47" s="120"/>
-      <c r="M47" s="120"/>
-      <c r="N47" s="120"/>
-      <c r="O47" s="120"/>
-      <c r="P47" s="120"/>
-      <c r="Q47" s="120"/>
-      <c r="R47" s="120"/>
-      <c r="S47" s="120"/>
-      <c r="T47" s="120"/>
-      <c r="U47" s="120"/>
-      <c r="V47" s="120"/>
-      <c r="W47" s="120"/>
-      <c r="X47" s="120"/>
-      <c r="Y47" s="120"/>
-      <c r="Z47" s="120"/>
-      <c r="AA47" s="120"/>
-      <c r="AB47" s="120"/>
-      <c r="AC47" s="120"/>
-      <c r="AD47" s="120"/>
-      <c r="AE47" s="120"/>
-      <c r="AF47" s="120"/>
-      <c r="AG47" s="120"/>
-      <c r="AH47" s="120"/>
-      <c r="AI47" s="120"/>
-      <c r="AJ47" s="120"/>
-      <c r="AK47" s="120"/>
-      <c r="AL47" s="120"/>
-      <c r="AM47" s="120"/>
-      <c r="AN47" s="120"/>
-      <c r="AO47" s="120"/>
-      <c r="AP47" s="120"/>
-      <c r="AQ47" s="120"/>
-      <c r="AR47" s="120"/>
-      <c r="AS47" s="120"/>
-      <c r="AT47" s="120"/>
-      <c r="AU47" s="120"/>
-      <c r="AV47" s="120"/>
-      <c r="AW47" s="120"/>
-      <c r="AX47" s="120"/>
-      <c r="AY47" s="120"/>
-      <c r="AZ47" s="120"/>
-      <c r="BA47" s="120"/>
-    </row>
-    <row r="48" spans="1:53" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="73"/>
+      <c r="G47" s="89" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="76"/>
       <c r="B48" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C48" s="76">
+      <c r="C48" s="79">
         <v>171397002</v>
       </c>
-      <c r="D48" s="56" t="s">
+      <c r="D48" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="104">
+      <c r="E48" s="58">
         <v>13848</v>
       </c>
-      <c r="F48" s="57">
+      <c r="F48" s="59">
         <f t="shared" si="3"/>
         <v>3.9903450248022072E-4</v>
       </c>
-      <c r="G48" s="121"/>
-      <c r="H48" s="120"/>
-      <c r="I48" s="120"/>
-      <c r="J48" s="120"/>
-      <c r="K48" s="120"/>
-      <c r="L48" s="120"/>
-      <c r="M48" s="120"/>
-      <c r="N48" s="120"/>
-      <c r="O48" s="120"/>
-      <c r="P48" s="120"/>
-      <c r="Q48" s="120"/>
-      <c r="R48" s="120"/>
-      <c r="S48" s="120"/>
-      <c r="T48" s="120"/>
-      <c r="U48" s="120"/>
-      <c r="V48" s="120"/>
-      <c r="W48" s="120"/>
-      <c r="X48" s="120"/>
-      <c r="Y48" s="120"/>
-      <c r="Z48" s="120"/>
-      <c r="AA48" s="120"/>
-      <c r="AB48" s="120"/>
-      <c r="AC48" s="120"/>
-      <c r="AD48" s="120"/>
-      <c r="AE48" s="120"/>
-      <c r="AF48" s="120"/>
-      <c r="AG48" s="120"/>
-      <c r="AH48" s="120"/>
-      <c r="AI48" s="120"/>
-      <c r="AJ48" s="120"/>
-      <c r="AK48" s="120"/>
-      <c r="AL48" s="120"/>
-      <c r="AM48" s="120"/>
-      <c r="AN48" s="120"/>
-      <c r="AO48" s="120"/>
-      <c r="AP48" s="120"/>
-      <c r="AQ48" s="120"/>
-      <c r="AR48" s="120"/>
-      <c r="AS48" s="120"/>
-      <c r="AT48" s="120"/>
-      <c r="AU48" s="120"/>
-      <c r="AV48" s="120"/>
-      <c r="AW48" s="120"/>
-      <c r="AX48" s="120"/>
-      <c r="AY48" s="120"/>
-      <c r="AZ48" s="120"/>
-      <c r="BA48" s="120"/>
-    </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A49" s="74"/>
+      <c r="G48" s="89"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="77"/>
       <c r="B49" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C49" s="39">
+        <v>153</v>
+      </c>
+      <c r="C49" s="41">
         <v>182777000</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="93">
+      <c r="E49" s="20">
         <f>479817</f>
         <v>479817</v>
       </c>
@@ -3115,137 +2540,91 @@
         <f t="shared" si="3"/>
         <v>1.3826078702812831E-2</v>
       </c>
-      <c r="G49" s="119"/>
-      <c r="H49" s="122"/>
-      <c r="I49" s="122"/>
-      <c r="J49" s="122"/>
-      <c r="K49" s="122"/>
-      <c r="L49" s="122"/>
-      <c r="M49" s="122"/>
-      <c r="N49" s="122"/>
-      <c r="O49" s="122"/>
-      <c r="P49" s="122"/>
-      <c r="Q49" s="122"/>
-      <c r="R49" s="122"/>
-      <c r="S49" s="122"/>
-      <c r="T49" s="122"/>
-      <c r="U49" s="122"/>
-      <c r="V49" s="122"/>
-      <c r="W49" s="122"/>
-      <c r="X49" s="122"/>
-      <c r="Y49" s="122"/>
-      <c r="Z49" s="122"/>
-      <c r="AA49" s="122"/>
-      <c r="AB49" s="122"/>
-      <c r="AC49" s="122"/>
-      <c r="AD49" s="122"/>
-      <c r="AE49" s="122"/>
-      <c r="AF49" s="122"/>
-      <c r="AG49" s="122"/>
-      <c r="AH49" s="122"/>
-      <c r="AI49" s="122"/>
-      <c r="AJ49" s="122"/>
-      <c r="AK49" s="122"/>
-      <c r="AL49" s="122"/>
-      <c r="AM49" s="122"/>
-      <c r="AN49" s="122"/>
-      <c r="AO49" s="122"/>
-      <c r="AP49" s="122"/>
-      <c r="AQ49" s="122"/>
-      <c r="AR49" s="122"/>
-      <c r="AS49" s="122"/>
-      <c r="AT49" s="122"/>
-      <c r="AU49" s="122"/>
-      <c r="AV49" s="122"/>
-      <c r="AW49" s="122"/>
-      <c r="AX49" s="122"/>
-      <c r="AY49" s="122"/>
-      <c r="AZ49" s="122"/>
-      <c r="BA49" s="122"/>
-    </row>
-    <row r="50" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A50" s="63"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="92"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="116"/>
-    </row>
-    <row r="51" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="65"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="C51" s="34">
+      <c r="C51" s="35">
         <v>23852006</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="100">
+      <c r="E51" s="36">
         <f>1324893+32275</f>
         <v>1357168</v>
       </c>
-      <c r="F51" s="36">
+      <c r="F51" s="37">
         <f>E51/$E$8</f>
         <v>3.9107225423315732E-2</v>
       </c>
-      <c r="G51" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="52" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G51" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="19">
         <v>268400002</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="93">
+      <c r="E52" s="20">
         <v>3640582</v>
       </c>
       <c r="F52" s="8">
         <f>E52/$E$8</f>
         <v>0.10490452246594793</v>
       </c>
-      <c r="G52" s="13"/>
-    </row>
-    <row r="53" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="G52" s="14"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="19">
         <v>428803005</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E53" s="93">
+      <c r="E53" s="20">
         <v>2912978</v>
       </c>
       <c r="F53" s="8">
         <f>E53/$E$8</f>
         <v>8.3938382940917711E-2</v>
       </c>
-      <c r="G53" s="13"/>
-    </row>
-    <row r="54" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B54" s="17" t="s">
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B54" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C54" s="19">
         <v>29303009</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E54" s="93">
+      <c r="E54" s="20">
         <f>24176+11891+10525</f>
         <v>46592</v>
       </c>
@@ -3253,185 +2632,185 @@
         <f>E54/$E$8</f>
         <v>1.3425632249825566E-3</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="55" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B55" s="17" t="s">
+      <c r="G54" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B55" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="19">
         <v>46825001</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="E55" s="93">
+      <c r="E55" s="20">
         <v>836431</v>
       </c>
       <c r="F55" s="8">
         <f>E55/$E$8</f>
         <v>2.410202397053968E-2</v>
       </c>
-      <c r="G55" s="13"/>
-    </row>
-    <row r="56" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A56" s="63"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="65"/>
-      <c r="E56" s="92"/>
-      <c r="F56" s="66"/>
-      <c r="G56" s="13"/>
-    </row>
-    <row r="57" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A57" s="72" t="s">
+      <c r="G55" s="14"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="65"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="45" t="s">
+      <c r="B57" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="44">
+      <c r="C57" s="46">
         <v>250980009</v>
       </c>
-      <c r="D57" s="45" t="s">
+      <c r="D57" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E57" s="97">
+      <c r="E57" s="47">
         <v>4854</v>
       </c>
       <c r="F57" s="8">
         <f t="shared" ref="F57" si="4">E57/$E$8</f>
         <v>1.3986954614666317E-4</v>
       </c>
-      <c r="G57" s="13"/>
-    </row>
-    <row r="58" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B58" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="18">
+      <c r="G57" s="14"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B58" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="19">
         <v>429283006</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E58" s="93">
+      <c r="E58" s="20">
         <v>40260</v>
       </c>
       <c r="F58" s="8">
         <f t="shared" ref="F58:F63" si="5">E58/$E$8</f>
         <v>1.1601046410928428E-3</v>
       </c>
-      <c r="G58" s="13"/>
-    </row>
-    <row r="59" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B59" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="C59" s="18">
+      <c r="G58" s="14"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B59" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" s="19">
         <v>89666000</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E59" s="93">
+      <c r="E59" s="20">
         <v>142227</v>
       </c>
       <c r="F59" s="8">
         <f t="shared" si="5"/>
         <v>4.0983160156162881E-3</v>
       </c>
-      <c r="G59" s="13"/>
-    </row>
-    <row r="60" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B60" s="29" t="s">
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B60" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="48">
+      <c r="C60" s="50">
         <v>233169004</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="E60" s="105">
+      <c r="E60" s="22">
         <v>5386</v>
       </c>
       <c r="F60" s="8">
         <f t="shared" si="5"/>
         <v>1.5519929450884379E-4</v>
       </c>
-      <c r="G60" s="13"/>
-    </row>
-    <row r="61" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B61" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C61" s="39">
+      <c r="G60" s="14"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B61" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" s="41">
         <v>426220008</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E61" s="93">
+      <c r="E61" s="20">
         <v>41331</v>
       </c>
       <c r="F61" s="8">
         <f t="shared" si="5"/>
         <v>1.1909658450324958E-3</v>
       </c>
-      <c r="G61" s="13"/>
-    </row>
-    <row r="62" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B62" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="C62" s="39">
+      <c r="G61" s="14"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B62" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" s="41">
         <v>386237008</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E62" s="93">
+      <c r="E62" s="20">
         <v>12504</v>
       </c>
       <c r="F62" s="8">
         <f t="shared" si="5"/>
         <v>3.6030671714418547E-4</v>
       </c>
-      <c r="G62" s="13"/>
-    </row>
-    <row r="63" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B63" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="49">
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B63" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" s="51">
         <v>18590009</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D63" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="106">
+      <c r="E63" s="28">
         <v>11415</v>
       </c>
       <c r="F63" s="8">
         <f t="shared" si="5"/>
         <v>3.2892683750806756E-4</v>
       </c>
-      <c r="G63" s="13"/>
-    </row>
-    <row r="64" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="B64" s="28" t="s">
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B64" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C64" s="23">
+      <c r="C64" s="24">
         <v>128968000</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E64" s="99">
+      <c r="E64" s="7">
         <v>11121</v>
       </c>
       <c r="F64" s="8">
@@ -3439,28 +2818,28 @@
         <v>3.2045513446580983E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="63"/>
-      <c r="B65" s="62"/>
-      <c r="C65" s="64"/>
-      <c r="D65" s="65"/>
-      <c r="E65" s="92"/>
-      <c r="F65" s="66"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" s="65"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
+      <c r="F65" s="68"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="C66" s="23">
+      <c r="C66" s="24">
         <v>228621007</v>
       </c>
-      <c r="D66" s="45" t="s">
+      <c r="D66" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E66" s="97">
+      <c r="E66" s="47">
         <v>16170</v>
       </c>
       <c r="F66" s="8">
@@ -3468,17 +2847,17 @@
         <v>4.6594366732417456E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B67" s="31" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B67" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="C67" s="23">
+      <c r="C67" s="24">
         <v>431774007</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E67" s="99">
+      <c r="E67" s="7">
         <f>90201+18244+5020</f>
         <v>113465</v>
       </c>
@@ -3487,20 +2866,20 @@
         <v>3.2695298832985447E-3</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B68" s="31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B68" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="C68" s="23">
+      <c r="C68" s="24">
         <v>431949004</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E68" s="99">
+      <c r="E68" s="7">
         <v>17139</v>
       </c>
       <c r="F68" s="8">
@@ -3508,28 +2887,28 @@
         <v>4.9386570898386068E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="63"/>
-      <c r="B69" s="62"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="92"/>
-      <c r="F69" s="66"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69" s="65"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="67"/>
+      <c r="F69" s="68"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B70" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C70" s="25">
+      <c r="B70" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="26">
         <v>87750000</v>
       </c>
-      <c r="D70" s="26" t="s">
+      <c r="D70" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E70" s="99">
+      <c r="E70" s="7">
         <v>6252</v>
       </c>
       <c r="F70" s="8">
@@ -3537,17 +2916,17 @@
         <v>1.8015335857209273E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B71" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C71" s="18">
+        <v>148</v>
+      </c>
+      <c r="C71" s="19">
         <v>235425002</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="D71" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E71" s="107">
+      <c r="E71" s="31">
         <v>6963</v>
       </c>
       <c r="F71" s="8">
@@ -3555,50 +2934,50 @@
         <v>2.0064104858245069E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="63"/>
-      <c r="B72" s="62"/>
-      <c r="C72" s="64"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="92"/>
-      <c r="F72" s="66"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A72" s="65"/>
+      <c r="B72" s="64"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="67"/>
+      <c r="F72" s="68"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B73" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="C73" s="34">
+      <c r="B73" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="35">
         <v>33747003</v>
       </c>
-      <c r="D73" s="35" t="s">
+      <c r="D73" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E73" s="108">
+      <c r="E73" s="39">
         <f>829194+257616+146229+111713+79687+9786+5904+116651</f>
         <v>1556780</v>
       </c>
-      <c r="F73" s="36">
+      <c r="F73" s="37">
         <f>E73/$E$8</f>
         <v>4.4859108374578134E-2</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B74" s="17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B74" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C74" s="18">
+      <c r="C74" s="19">
         <v>386328006</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D74" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E74" s="107">
+      <c r="E74" s="31">
         <v>6379</v>
       </c>
       <c r="F74" s="8">
@@ -3606,28 +2985,28 @@
         <v>1.838129037638163E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A75" s="63"/>
-      <c r="B75" s="62"/>
-      <c r="C75" s="64"/>
-      <c r="D75" s="65"/>
-      <c r="E75" s="92"/>
-      <c r="F75" s="66"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A75" s="65"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="67"/>
+      <c r="E75" s="67"/>
+      <c r="F75" s="68"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B76" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="C76" s="18">
+      <c r="C76" s="19">
         <v>49689007</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E76" s="93">
+      <c r="E76" s="20">
         <v>225923</v>
       </c>
       <c r="F76" s="8">
@@ -3635,17 +3014,17 @@
         <v>6.5100427429115332E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B77" s="17" t="s">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B77" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="C77" s="18">
+      <c r="C77" s="19">
         <v>182556001</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E77" s="93">
+      <c r="E77" s="20">
         <v>8887</v>
       </c>
       <c r="F77" s="8">
@@ -3653,17 +3032,17 @@
         <v>2.5608171747123928E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B78" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C78" s="18">
+      <c r="C78" s="19">
         <v>79321009</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="D78" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E78" s="93">
+      <c r="E78" s="20">
         <v>181145</v>
       </c>
       <c r="F78" s="8">
@@ -3671,18 +3050,18 @@
         <v>5.2197505020060361E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C79" s="18">
+      <c r="C79" s="19">
         <v>302488007</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E79" s="93">
+      <c r="E79" s="20">
         <v>5548</v>
       </c>
       <c r="F79" s="8">
@@ -3695,28 +3074,28 @@
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A80" s="63"/>
-      <c r="B80" s="62"/>
-      <c r="C80" s="64"/>
-      <c r="D80" s="65"/>
-      <c r="E80" s="92"/>
-      <c r="F80" s="66"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A80" s="65"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="67"/>
+      <c r="E80" s="67"/>
+      <c r="F80" s="68"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B81" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="C81" s="46">
+      <c r="C81" s="48">
         <v>78086002</v>
       </c>
-      <c r="D81" s="47" t="s">
+      <c r="D81" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="109">
+      <c r="E81" s="49">
         <v>12632</v>
       </c>
       <c r="F81" s="8">
@@ -3724,17 +3103,17 @@
         <v>3.6399507765237931E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B82" s="17" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B82" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="C82" s="18">
+      <c r="C82" s="19">
         <v>409582008</v>
       </c>
-      <c r="D82" s="19" t="s">
+      <c r="D82" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E82" s="93">
+      <c r="E82" s="20">
         <v>10513</v>
       </c>
       <c r="F82" s="8">
@@ -3742,36 +3121,39 @@
         <v>3.0293542205188915E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="77"/>
-      <c r="B83" s="32" t="s">
+    <row r="83" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="80"/>
+      <c r="B83" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="C83" s="78">
+      <c r="C83" s="81">
         <v>182705007</v>
       </c>
-      <c r="D83" s="79" t="s">
+      <c r="D83" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="E83" s="110">
+      <c r="E83" s="82">
         <v>5703</v>
       </c>
-      <c r="F83" s="80">
+      <c r="F83" s="83">
         <f t="shared" si="7"/>
         <v>1.643337498299176E-4</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B84" s="17" t="s">
+      <c r="G83" s="55" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B84" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C84" s="46">
+      <c r="C84" s="48">
         <v>22633006</v>
       </c>
-      <c r="D84" s="47" t="s">
+      <c r="D84" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="E84" s="109">
+      <c r="E84" s="49">
         <v>72</v>
       </c>
       <c r="F84" s="8">
@@ -3779,28 +3161,28 @@
         <v>2.0747027858590333E-6</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="63"/>
-      <c r="B85" s="62"/>
-      <c r="C85" s="64"/>
-      <c r="D85" s="65"/>
-      <c r="E85" s="92"/>
-      <c r="F85" s="66"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="65"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="66"/>
+      <c r="D85" s="67"/>
+      <c r="E85" s="67"/>
+      <c r="F85" s="68"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B86" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B86" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C86" s="18">
+      <c r="C86" s="19">
         <v>423184003</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E86" s="93">
+      <c r="E86" s="20">
         <v>233392</v>
       </c>
       <c r="F86" s="8">
@@ -3808,17 +3190,17 @@
         <v>6.7252643416279376E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B87" s="17" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B87" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="C87" s="18">
+      <c r="C87" s="19">
         <v>423401003</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E87" s="93">
+      <c r="E87" s="20">
         <v>9079</v>
       </c>
       <c r="F87" s="8">
@@ -3826,17 +3208,17 @@
         <v>2.6161425823353007E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B88" s="17" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B88" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C88" s="18">
+      <c r="C88" s="19">
         <v>225399009</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D88" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E88" s="93">
+      <c r="E88" s="20">
         <f>81183+23883</f>
         <v>105066</v>
       </c>
@@ -3845,20 +3227,20 @@
         <v>3.0275100402647943E-3</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B89" s="17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B89" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C89" s="18">
+      <c r="C89" s="19">
         <v>278414003</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E89" s="93">
+      <c r="E89" s="20">
         <v>8606</v>
       </c>
       <c r="F89" s="8">
@@ -3866,28 +3248,28 @@
         <v>2.4798461354309499E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="63"/>
-      <c r="B90" s="62"/>
-      <c r="C90" s="64"/>
-      <c r="D90" s="65"/>
-      <c r="E90" s="92"/>
-      <c r="F90" s="66"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="65"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="66"/>
+      <c r="D90" s="67"/>
+      <c r="E90" s="67"/>
+      <c r="F90" s="68"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="B91" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B91" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C91" s="18">
+      <c r="C91" s="19">
         <v>58715004</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E91" s="93">
+      <c r="E91" s="20">
         <v>500129</v>
       </c>
       <c r="F91" s="8">
@@ -3895,17 +3277,17 @@
         <v>1.441137541095684E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B92" s="17" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B92" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="C92" s="18">
+      <c r="C92" s="19">
         <v>56469005</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E92" s="93">
+      <c r="E92" s="20">
         <v>48867</v>
       </c>
       <c r="F92" s="8">
@@ -3913,17 +3295,17 @@
         <v>1.4081180699524081E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B93" s="17" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B93" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="C93" s="46">
+      <c r="C93" s="48">
         <v>225287004</v>
       </c>
-      <c r="D93" s="47" t="s">
+      <c r="D93" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="E93" s="109">
+      <c r="E93" s="49">
         <f>3074+5551+2531</f>
         <v>11156</v>
       </c>
@@ -3932,20 +3314,20 @@
         <v>3.2146367054226908E-4</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B94" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C94" s="23">
+      <c r="C94" s="24">
         <v>386423001</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E94" s="99">
+      <c r="E94" s="7">
         <v>118152</v>
       </c>
       <c r="F94" s="8">
@@ -3953,28 +3335,28 @@
         <v>3.4045872715946736E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="63"/>
-      <c r="B95" s="62"/>
-      <c r="C95" s="64"/>
-      <c r="D95" s="65"/>
-      <c r="E95" s="92"/>
-      <c r="F95" s="66"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="65"/>
+      <c r="B95" s="64"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="67"/>
+      <c r="E95" s="67"/>
+      <c r="F95" s="68"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C96" s="18">
+      <c r="C96" s="19">
         <v>398041008</v>
       </c>
-      <c r="D96" s="19" t="s">
+      <c r="D96" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E96" s="93">
+      <c r="E96" s="20">
         <v>267096</v>
       </c>
       <c r="F96" s="8">
@@ -3982,17 +3364,17 @@
         <v>7.6964557679417272E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B97" s="17" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B97" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="18">
+      <c r="C97" s="19">
         <v>449199004</v>
       </c>
-      <c r="D97" s="19" t="s">
+      <c r="D97" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E97" s="93">
+      <c r="E97" s="20">
         <v>15242</v>
       </c>
       <c r="F97" s="8">
@@ -4000,17 +3382,17 @@
         <v>4.3920305363976926E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B98" s="17" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B98" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="18">
+      <c r="C98" s="19">
         <v>426498007</v>
       </c>
-      <c r="D98" s="19" t="s">
+      <c r="D98" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E98" s="93">
+      <c r="E98" s="20">
         <v>177218</v>
       </c>
       <c r="F98" s="8">
@@ -4018,36 +3400,36 @@
         <v>5.1065927542273074E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B99" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C99" s="18">
+      <c r="C99" s="19">
         <v>445828009</v>
       </c>
-      <c r="D99" s="19" t="s">
+      <c r="D99" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E99" s="93">
+      <c r="E99" s="20">
         <v>23035</v>
       </c>
       <c r="F99" s="8">
         <f t="shared" si="8"/>
         <v>6.637608148925393E-4</v>
       </c>
-      <c r="G99" s="20"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G99" s="21"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B100" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C100" s="18">
+      <c r="C100" s="19">
         <v>284405008</v>
       </c>
-      <c r="D100" s="19" t="s">
+      <c r="D100" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E100" s="93">
+      <c r="E100" s="20">
         <v>23362</v>
       </c>
       <c r="F100" s="8">
@@ -4055,17 +3437,17 @@
         <v>6.7318342337831575E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B101" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C101" s="18">
+      <c r="C101" s="19">
         <v>284394000</v>
       </c>
-      <c r="D101" s="19" t="s">
+      <c r="D101" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E101" s="93">
+      <c r="E101" s="20">
         <v>6821</v>
       </c>
       <c r="F101" s="8">
@@ -4073,28 +3455,28 @@
         <v>1.9654927364367314E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="63"/>
-      <c r="B102" s="62"/>
-      <c r="C102" s="64"/>
-      <c r="D102" s="65"/>
-      <c r="E102" s="92"/>
-      <c r="F102" s="66"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="65"/>
+      <c r="B102" s="64"/>
+      <c r="C102" s="66"/>
+      <c r="D102" s="67"/>
+      <c r="E102" s="67"/>
+      <c r="F102" s="68"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C103" s="18">
+      <c r="C103" s="19">
         <v>304562007</v>
       </c>
-      <c r="D103" s="19" t="s">
+      <c r="D103" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E103" s="93">
+      <c r="E103" s="20">
         <v>1222966</v>
       </c>
       <c r="F103" s="8">
@@ -4102,17 +3484,17 @@
         <v>3.5240152322373312E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B104" s="17" t="s">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B104" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="C104" s="18">
+      <c r="C104" s="19">
         <v>429202003</v>
       </c>
-      <c r="D104" s="19" t="s">
+      <c r="D104" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="E104" s="93">
+      <c r="E104" s="20">
         <v>7142</v>
       </c>
       <c r="F104" s="8">
@@ -4120,17 +3502,17 @@
         <v>2.05798990230628E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B105" s="17" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B105" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="C105" s="18">
+      <c r="C105" s="19">
         <v>308292007</v>
       </c>
-      <c r="D105" s="19" t="s">
+      <c r="D105" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E105" s="93">
+      <c r="E105" s="20">
         <v>49518</v>
       </c>
       <c r="F105" s="8">
@@ -4138,28 +3520,28 @@
         <v>1.4268768409745501E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="63"/>
-      <c r="B106" s="62"/>
-      <c r="C106" s="64"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="92"/>
-      <c r="F106" s="66"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="65"/>
+      <c r="B106" s="64"/>
+      <c r="C106" s="66"/>
+      <c r="D106" s="67"/>
+      <c r="E106" s="67"/>
+      <c r="F106" s="68"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B107" s="28" t="s">
+      <c r="B107" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C107" s="18">
+      <c r="C107" s="19">
         <v>392247006</v>
       </c>
-      <c r="D107" s="19" t="s">
+      <c r="D107" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E107" s="93">
+      <c r="E107" s="20">
         <v>14311</v>
       </c>
       <c r="F107" s="8">
@@ -4167,17 +3549,17 @@
         <v>4.123759940059531E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B108" s="28" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B108" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="18">
+      <c r="C108" s="19">
         <v>226005007</v>
       </c>
-      <c r="D108" s="19" t="s">
+      <c r="D108" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E108" s="93">
+      <c r="E108" s="20">
         <v>6662</v>
       </c>
       <c r="F108" s="8">
@@ -4185,17 +3567,17 @@
         <v>1.919676383249011E-4</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B109" s="17" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B109" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="C109" s="18">
+      <c r="C109" s="19">
         <v>425074000</v>
       </c>
-      <c r="D109" s="19" t="s">
+      <c r="D109" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E109" s="93">
+      <c r="E109" s="20">
         <v>54225</v>
       </c>
       <c r="F109" s="8">
@@ -4203,17 +3585,17 @@
         <v>1.5625105356000845E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B110" s="28" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B110" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C110" s="18">
+      <c r="C110" s="19">
         <v>430824005</v>
       </c>
-      <c r="D110" s="19" t="s">
+      <c r="D110" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E110" s="93">
+      <c r="E110" s="20">
         <v>139261</v>
       </c>
       <c r="F110" s="8">
@@ -4221,17 +3603,17 @@
         <v>4.0128497869654839E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B111" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C111" s="18">
+      <c r="C111" s="19">
         <v>392230005</v>
       </c>
-      <c r="D111" s="19" t="s">
+      <c r="D111" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E111" s="93">
+      <c r="E111" s="20">
         <f>6832761+117764+283620</f>
         <v>7234145</v>
       </c>
@@ -4240,20 +3622,20 @@
         <v>0.2084541775667805</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B112" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="C112" s="18">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B112" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="C112" s="19">
         <v>353008</v>
       </c>
-      <c r="D112" s="19" t="s">
+      <c r="D112" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E112" s="93">
+      <c r="E112" s="20">
         <f>98895+9635+10390</f>
         <v>118920</v>
       </c>
@@ -4262,20 +3644,20 @@
         <v>3.4267174346438367E-3</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B113" s="31" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B113" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="C113" s="18">
+      <c r="C113" s="19">
         <v>424287005</v>
       </c>
-      <c r="D113" s="19" t="s">
+      <c r="D113" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E113" s="93">
+      <c r="E113" s="20">
         <v>10238</v>
       </c>
       <c r="F113" s="8">
@@ -4283,17 +3665,17 @@
         <v>2.9501121002256642E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B114" s="28" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B114" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="C114" s="18">
+      <c r="C114" s="19">
         <v>396540005</v>
       </c>
-      <c r="D114" s="19" t="s">
+      <c r="D114" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E114" s="93">
+      <c r="E114" s="20">
         <f>178456+6390</f>
         <v>184846</v>
       </c>
@@ -4302,20 +3684,20 @@
         <v>5.3263959882624843E-3</v>
       </c>
       <c r="G114" s="10" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B115" s="29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B115" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="C115" s="18">
+      <c r="C115" s="19">
         <v>405427009</v>
       </c>
-      <c r="D115" s="19" t="s">
+      <c r="D115" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E115" s="93">
+      <c r="E115" s="20">
         <v>22791</v>
       </c>
       <c r="F115" s="8">
@@ -4323,29 +3705,29 @@
         <v>6.5672987767379485E-4</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="63"/>
-      <c r="B116" s="62"/>
-      <c r="C116" s="64"/>
-      <c r="D116" s="65"/>
-      <c r="E116" s="92"/>
-      <c r="F116" s="66"/>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116" s="65"/>
+      <c r="B116" s="64"/>
+      <c r="C116" s="66"/>
+      <c r="D116" s="67"/>
+      <c r="E116" s="67"/>
+      <c r="F116" s="68"/>
       <c r="G116" s="11"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B117" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C117" s="39">
+        <v>128</v>
+      </c>
+      <c r="B117" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C117" s="41">
         <v>46973005</v>
       </c>
-      <c r="D117" s="19" t="s">
+      <c r="D117" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E117" s="93">
+      <c r="E117" s="20">
         <f>95714+6174</f>
         <v>101888</v>
       </c>
@@ -4354,24 +3736,27 @@
         <v>2.9359349645222944E-3</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B118" s="17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B118" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C118" s="42">
+        <v>248753002</v>
+      </c>
+      <c r="D118" s="43" t="s">
+        <v>252</v>
+      </c>
+      <c r="E118" s="28"/>
+      <c r="G118" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C118" s="40">
-        <v>248753002</v>
-      </c>
-      <c r="D118" s="41" t="s">
-        <v>251</v>
-      </c>
-      <c r="E118" s="106"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B119" s="17" t="s">
-        <v>172</v>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B119" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="C119" s="6">
         <v>68664003</v>
@@ -4379,7 +3764,7 @@
       <c r="D119" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E119" s="99">
+      <c r="E119" s="7">
         <v>8705</v>
       </c>
       <c r="F119" s="8">
@@ -4387,9 +3772,9 @@
         <v>2.5083732987365119E-4</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B120" s="17" t="s">
-        <v>174</v>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B120" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="C120" s="6">
         <v>65653002</v>
@@ -4397,7 +3782,7 @@
       <c r="D120" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E120" s="99">
+      <c r="E120" s="7">
         <v>6058</v>
       </c>
       <c r="F120" s="8">
@@ -4405,9 +3790,9 @@
         <v>1.7456318717686144E-4</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B121" s="17" t="s">
-        <v>175</v>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B121" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="C121" s="6">
         <v>252465000</v>
@@ -4415,7 +3800,7 @@
       <c r="D121" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E121" s="99">
+      <c r="E121" s="7">
         <f>1350281+105463+5371</f>
         <v>1461115</v>
       </c>
@@ -4424,20 +3809,20 @@
         <v>4.2102491124450296E-2</v>
       </c>
       <c r="G121" s="10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B122" s="17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B122" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="C122" s="44">
+      <c r="C122" s="46">
         <v>408867002</v>
       </c>
-      <c r="D122" s="45" t="s">
+      <c r="D122" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E122" s="97">
+      <c r="E122" s="47">
         <v>5287</v>
       </c>
       <c r="F122" s="8">
@@ -4445,8 +3830,8 @@
         <v>1.5234657817828762E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B123" s="17" t="s">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B123" s="18" t="s">
         <v>211</v>
       </c>
       <c r="C123" s="6">
@@ -4455,7 +3840,7 @@
       <c r="D123" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E123" s="99">
+      <c r="E123" s="7">
         <f>53137+7590</f>
         <v>60727</v>
       </c>
@@ -4464,11 +3849,11 @@
         <v>1.7498677232897432E-3</v>
       </c>
       <c r="G123" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B124" s="17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B124" s="18" t="s">
         <v>212</v>
       </c>
       <c r="C124" s="6">
@@ -4477,7 +3862,7 @@
       <c r="D124" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E124" s="99">
+      <c r="E124" s="7">
         <v>224458</v>
       </c>
       <c r="F124" s="8">
@@ -4485,7 +3870,7 @@
         <v>6.4678283042825958E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B125" s="5" t="s">
         <v>213</v>
       </c>
@@ -4495,7 +3880,7 @@
       <c r="D125" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E125" s="99">
+      <c r="E125" s="7">
         <v>214517</v>
       </c>
       <c r="F125" s="8">
@@ -4503,28 +3888,28 @@
         <v>6.1813752432516977E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="63"/>
-      <c r="B126" s="62"/>
-      <c r="C126" s="64"/>
-      <c r="D126" s="65"/>
-      <c r="E126" s="92"/>
-      <c r="F126" s="66"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126" s="65"/>
+      <c r="B126" s="64"/>
+      <c r="C126" s="66"/>
+      <c r="D126" s="67"/>
+      <c r="E126" s="67"/>
+      <c r="F126" s="68"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B127" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C127" s="18">
+        <v>129</v>
+      </c>
+      <c r="B127" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C127" s="19">
         <v>447686008</v>
       </c>
-      <c r="D127" s="30" t="s">
+      <c r="D127" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="E127" s="99">
+      <c r="E127" s="7">
         <v>6325</v>
       </c>
       <c r="F127" s="8">
@@ -4532,17 +3917,17 @@
         <v>1.8225687667442202E-4</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B128" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C128" s="18">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B128" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C128" s="19">
         <v>182555002</v>
       </c>
-      <c r="D128" s="30" t="s">
+      <c r="D128" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E128" s="99">
+      <c r="E128" s="7">
         <v>77272</v>
       </c>
       <c r="F128" s="8">
@@ -4550,17 +3935,17 @@
         <v>2.226617134290267E-3</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B129" s="17" t="s">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B129" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="C129" s="18">
+      <c r="C129" s="19">
         <v>373675000</v>
       </c>
-      <c r="D129" s="30" t="s">
+      <c r="D129" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E129" s="99">
+      <c r="E129" s="7">
         <v>9886</v>
       </c>
       <c r="F129" s="8">
@@ -4568,17 +3953,17 @@
         <v>2.8486821862503336E-4</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B130" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C130" s="18">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B130" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C130" s="19">
         <v>133901003</v>
       </c>
-      <c r="D130" s="30" t="s">
+      <c r="D130" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E130" s="99">
+      <c r="E130" s="7">
         <v>14901</v>
       </c>
       <c r="F130" s="8">
@@ -4586,17 +3971,17 @@
         <v>4.2937703072340911E-4</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B131" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C131" s="18">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B131" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C131" s="19">
         <v>182531007</v>
       </c>
-      <c r="D131" s="38" t="s">
+      <c r="D131" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E131" s="111">
+      <c r="E131" s="27">
         <v>19308</v>
       </c>
       <c r="F131" s="8">
@@ -4604,17 +3989,17 @@
         <v>5.5636613040786406E-4</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B132" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C132" s="18">
+      <c r="C132" s="19">
         <v>22206003</v>
       </c>
-      <c r="D132" s="42" t="s">
+      <c r="D132" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="E132" s="93">
+      <c r="E132" s="20">
         <v>6209</v>
       </c>
       <c r="F132" s="8">
@@ -4622,17 +4007,17 @@
         <v>1.7891429996387136E-4</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B133" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C133" s="18">
+      <c r="C133" s="19">
         <v>26906007</v>
       </c>
-      <c r="D133" s="16" t="s">
+      <c r="D133" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E133" s="93">
+      <c r="E133" s="20">
         <v>79672</v>
       </c>
       <c r="F133" s="8">
@@ -4640,17 +4025,17 @@
         <v>2.2957738938189014E-3</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B134" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C134" s="18">
+        <v>165</v>
+      </c>
+      <c r="C134" s="19">
         <v>372045002</v>
       </c>
-      <c r="D134" s="42" t="s">
+      <c r="D134" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="E134" s="93">
+      <c r="E134" s="20">
         <v>32598</v>
       </c>
       <c r="F134" s="8">
@@ -4658,17 +4043,17 @@
         <v>9.3932168629767734E-4</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B135" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C135" s="18">
+        <v>167</v>
+      </c>
+      <c r="C135" s="19">
         <v>225116006</v>
       </c>
-      <c r="D135" s="42" t="s">
+      <c r="D135" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="E135" s="93">
+      <c r="E135" s="20">
         <v>13787</v>
       </c>
       <c r="F135" s="8">
@@ -4676,17 +4061,17 @@
         <v>3.9727676817553458E-4</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B136" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C136" s="18">
+      <c r="C136" s="19">
         <v>20655006</v>
       </c>
-      <c r="D136" s="42" t="s">
+      <c r="D136" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E136" s="93">
+      <c r="E136" s="20">
         <v>7266</v>
       </c>
       <c r="F136" s="8">
@@ -4694,17 +4079,17 @@
         <v>2.0937208947294076E-4</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B137" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C137" s="18">
+        <v>170</v>
+      </c>
+      <c r="C137" s="19">
         <v>225358003</v>
       </c>
-      <c r="D137" s="42" t="s">
+      <c r="D137" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E137" s="93">
+      <c r="E137" s="20">
         <v>177920</v>
       </c>
       <c r="F137" s="8">
@@ -4712,11 +4097,13 @@
         <v>5.126821106389433E-3</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E138" s="87">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E139" s="10">
+        <f>SUM(E11:E137)</f>
         <v>31253844</v>
       </c>
-      <c r="F138" s="115">
+      <c r="F139" s="8">
+        <f>SUM(F11:F137)</f>
         <v>0.90058940577227264</v>
       </c>
     </row>

</xml_diff>